<commit_message>
tidy up usage info in catalog-workflow work order template
</commit_message>
<xml_diff>
--- a/support/catalog-workflow-template.xlsx
+++ b/support/catalog-workflow-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgp/dl/dev/dot-doc/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0480A4D3-099F-004A-A130-1E35A861CAC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCFCC3-4F16-6943-8231-EC5D40FAC7F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <t>LABEL</t>
   </si>
   <si>
-    <t>v0.1.1</t>
+    <t>v0.1.2</t>
   </si>
 </sst>
 </file>
@@ -326,14 +326,8 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + LIB     : REQUIRED : Library. Typically this is NYU, but is important in multi-institutions projects, e.g., ACO.</a:t>
+            <a:t>    + LIB     : REQUIRED : Library. Typically this is NYU, but different values are used for multi-institution projects,</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -341,8 +335,14 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + BSN     : REQUIRED : Bibliographic System Number. The MARC 001 value.  The value in this column is used to link </a:t>
+            <a:t>                           e.g., AUB, AUC, PRINCETON, COLUMBIA, CORNELL.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -350,7 +350,7 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           descriptive metadata to the item, and to indicate items that are part of the same </a:t>
+            <a:t>    + BSN     : REQUIRED : Bibliographic System Number. This is the MARC 001 value.  The value in this column is used to </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -359,14 +359,8 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           intellectual entity, e.g., a multi-volume work.</a:t>
+            <a:t>                           link descriptive metadata to the item and to indicate items that are part of the same </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -374,8 +368,14 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + BARCODE : optional : helpful in large projects to correct digitization/mapping issues.</a:t>
+            <a:t>                           intellectual entity, e.g., a items in a multi-volume work.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -383,14 +383,8 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           Should be populated if TITLE is not provided.</a:t>
+            <a:t>    + BARCODE : optional : The barcode value is useful in large projects to resolve digitization/mapping issues.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -398,7 +392,16 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + DIGI_ID : GENERATED BY DLTS :</a:t>
+            <a:t>                           </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    + DIGI_ID : GENERATED BY DLTS (DO NOT FILL IN):</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -416,7 +419,7 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           The DIGI_ID value is used as a filename prefix for image files, </a:t>
+            <a:t>                           The DIGI_ID value is used as a filename prefix for digital files, </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -425,7 +428,7 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           e.g., ifa_egypt000001_n000023_d.tif</a:t>
+            <a:t>                           e.g., ifa_egypt000001_000023_d.tif</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -473,7 +476,7 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + TITLE   : REQUIRED : Title to facilitate digitization.</a:t>
+            <a:t>    + TITLE   : REQUIRED : This is the item title.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -556,23 +559,28 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>2.) Please fill in one row for each physical item that will be digitized</a:t>
+            <a:t>2.) Please fill in one row for each physical item that will be digitized.  Please do </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>not</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>3.) Please note that for multi-volume items, the LABEL column will be used to determine the display order of the items </a:t>
+            <a:t> fill in the DIGI_ID column.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -580,7 +588,16 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    when published.</a:t>
+            <a:t>3.) Please note that for multi-volume works, the LABEL column will be used to determine the display order of the digitized</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    items when published.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -927,7 +944,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2004,7 +2021,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update catalog-workflow-template.xlsx to v0.2.0
</commit_message>
<xml_diff>
--- a/support/catalog-workflow-template.xlsx
+++ b/support/catalog-workflow-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgp/dl/dev/dot-doc/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgp/Downloads/blorg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCFCC3-4F16-6943-8231-EC5D40FAC7F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80681F7-5BA0-2046-84E3-11C001D56E3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workorder" sheetId="5" r:id="rId1"/>
@@ -23,6 +23,256 @@
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0C22FDCC-8C60-7346-9B70-B1F2FF86C6A5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>REQUIRED</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Typically this value is NYU.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Please see "usage guide" tab for more information.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{62F9F602-22E9-A64D-B215-85D9BEB6A55C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>REQUIRED</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Please see "usage guide" tab for more information.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{2BF0E719-9E0A-B345-A9E3-0D4FC814C227}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPTIONAL</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, but very useful in large-scale digittization projects.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Please see "usage guide" tab for more information.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{DB921CCA-1E41-4348-97C2-8B6B21411E61}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>REQUIRED</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Please see "usage guide" tab for more information.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{FA6C7A8F-49BE-0643-B120-D95958FF63A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>REQUIRED IF APPLICABLE</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Please see "usage guide" tab for more information.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1862B8EE-71DD-5747-A243-DC95EE1CD1C9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RECOMMENDED</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Please see "usage guide" tab for more information.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -103,14 +353,14 @@
     <t>LABEL</t>
   </si>
   <si>
-    <t>v0.1.2</t>
+    <t>v0.2.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +383,46 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0432FF"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -178,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -203,6 +493,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,6 +512,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0432FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -233,8 +540,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>8467</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>59266</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -250,7 +557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="177800" y="63501"/>
-          <a:ext cx="9787467" cy="5905499"/>
+          <a:ext cx="9787467" cy="6227232"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -326,7 +633,41 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + LIB     : REQUIRED : Library. Typically this is NYU, but different values are used for multi-institution projects,</a:t>
+            <a:t>    + LIB     : </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>REQUIRED</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> : Library. Typically this is </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>NYU</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>, but different values are used for multi-institution projects,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -350,7 +691,24 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + BSN     : REQUIRED : Bibliographic System Number. This is the MARC 001 value.  The value in this column is used to </a:t>
+            <a:t>    + BSN     : </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>REQUIRED</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> : Bibliographic System Number. This is the MARC 001 value.  The value in this column is used to </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -401,7 +759,24 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + DIGI_ID : GENERATED BY DLTS (DO NOT FILL IN):</a:t>
+            <a:t>    + DIGI_ID : </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>REQUIRED</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> :</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -419,16 +794,76 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           The DIGI_ID value is used as a filename prefix for digital files, </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>                           e.g., ifa_egypt000001_000023_d.tif</a:t>
+            <a:t>                           e.g., </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ifa_egypt000001</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>                           The DIGI_ID value is </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>used as a filename prefix for </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>digital files, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>                           e.g., </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>ifa_egypt000001</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>_000023_d.tif</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -443,7 +878,24 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + LABEL   : REQUIRED IF RELEVANT : </a:t>
+            <a:t>    + LABEL   : </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>REQUIRED IF APPLICABLE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> : </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -461,7 +913,7 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>                           AND is used to order the items within the work.  </a:t>
+            <a:t>                           AND is used to order the items within the work during publication.  </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -476,7 +928,16 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    + TITLE   : REQUIRED : This is the item title.</a:t>
+            <a:t>    + TITLE   : RECOMMENDED : This is the item title.  The title allows the digitization team to confirm that the</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>                              physical object being digitized matches the information provided in the spreadsheet.  </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -939,20 +1400,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB841113-B6EC-8248-896A-BC61DC34FC72}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB841113-B6EC-8248-896A-BC61DC34FC72}">
   <dimension ref="A1:AI56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="115.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="35" width="28" style="9"/>
@@ -960,22 +1421,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1998,6 +2459,7 @@
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2005,7 +2467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08167E6-1A64-2D4D-9595-B2C7ABDF1343}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>